<commit_message>
refactor input to only collect input files, add regex for xlsx extension to filter non-xlsx files (ds.store) from hashSet of files pulled from the source folder
</commit_message>
<xml_diff>
--- a/src/input_trial_balances/TESTUS01.xlsx
+++ b/src/input_trial_balances/TESTUS01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Dev/Personal/Consolidation_Tool_Java/src/input_trial_balances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEDCD162-4BE8-2F44-AE85-80D874331187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B63E22-919A-0C49-A290-65C7D4A263DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27160" windowHeight="16440" xr2:uid="{7D95F7F2-E310-FE42-B6BB-709D674CF68E}"/>
+    <workbookView xWindow="700" yWindow="1000" windowWidth="27160" windowHeight="16440" xr2:uid="{7D95F7F2-E310-FE42-B6BB-709D674CF68E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trial_Balance" sheetId="1" r:id="rId1"/>
@@ -200,11 +200,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD61E748-E5AF-FC4B-AADF-7588769BCF54}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +540,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -559,379 +562,544 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
-        <v>20000</v>
+      <c r="C4" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>120</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
-        <v>15000</v>
+      <c r="C5" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>130</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
+      <c r="C6" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>135</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
-        <v>0</v>
+      <c r="C7" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>140</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
+      <c r="C8" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
+      <c r="C9" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>160</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2">
-        <v>0</v>
+      <c r="C10" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2">
-        <v>0</v>
+      <c r="C11" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>170</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2">
-        <v>0</v>
+      <c r="C12" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>175</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
+      <c r="C13" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>210</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2">
-        <v>-15500</v>
+      <c r="C14" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>220</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2">
-        <v>0</v>
+      <c r="C15" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>250</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2">
-        <v>0</v>
+      <c r="C16" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>300</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2">
-        <v>-10000</v>
+      <c r="C17" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>310</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2">
-        <v>0</v>
+      <c r="C18" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>330</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2">
-        <v>-2000</v>
+      <c r="C19" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>400</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2">
-        <v>-25000</v>
+      <c r="C20" s="3">
+        <v>-33000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>410</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2">
-        <v>0</v>
+      <c r="C21" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>415</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2">
-        <v>0</v>
+      <c r="C22" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>500</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="2">
-        <v>15000</v>
+      <c r="C23" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>510</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2">
-        <v>500</v>
+      <c r="C24" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="4">
         <v>520</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2">
-        <v>0</v>
+      <c r="C25" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="4">
         <v>530</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2">
-        <v>0</v>
+      <c r="C26" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="4">
         <v>535</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2">
-        <v>0</v>
+      <c r="C27" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>540</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2">
-        <v>0</v>
+      <c r="C28" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="4">
         <v>550</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="2">
-        <v>0</v>
+      <c r="C29" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="4">
         <v>560</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2">
-        <v>0</v>
+      <c r="C30" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="4">
         <v>570</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="4">
         <v>575</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="2">
-        <v>0</v>
+      <c r="C32" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="4">
         <v>580</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="2">
-        <v>0</v>
+      <c r="C33" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="4">
         <v>590</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="2">
-        <v>0</v>
+      <c r="C34" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="4">
         <v>595</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="2">
-        <v>0</v>
+      <c r="C35" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="4">
         <v>610</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="2">
-        <v>0</v>
-      </c>
+      <c r="C36" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="6"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="6"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" s="6"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" s="6"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" s="6"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" s="6"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" s="6"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>